<commit_message>
Renamed keys in dictionary
</commit_message>
<xml_diff>
--- a/party_list.xlsx
+++ b/party_list.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>email</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>John</t>

</xml_diff>